<commit_message>
Created test scripts filled form 'Write Your Review', 'Contact Us', and 'Subscription'. Clean comment and refolder all test scripts.
</commit_message>
<xml_diff>
--- a/cypress/fixtures/testCaseCriteria/testCaseCriteria_register.xlsx
+++ b/cypress/fixtures/testCaseCriteria/testCaseCriteria_register.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\awika-portfolio\automationexercise\cypress\fixtures\testCaseCriteria\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8B5A43-9504-47B1-B181-DF3E1309868A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB677BC-C502-4B25-B05D-1D7C0B702340}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1995" yWindow="-15000" windowWidth="25860" windowHeight="11880" tabRatio="553" activeTab="1" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
+    <workbookView xWindow="8460" yWindow="-13275" windowWidth="21525" windowHeight="10830" tabRatio="553" firstSheet="1" activeTab="8" xr2:uid="{63A55816-40FB-44DD-8B96-272E0273596B}"/>
   </bookViews>
   <sheets>
     <sheet name="column_ref" sheetId="20" r:id="rId1"/>
@@ -20,6 +20,8 @@
     <sheet name="reg_04" sheetId="24" r:id="rId5"/>
     <sheet name="reg_05" sheetId="25" r:id="rId6"/>
     <sheet name="reg_06" sheetId="26" r:id="rId7"/>
+    <sheet name="reg_07" sheetId="27" r:id="rId8"/>
+    <sheet name="reg_08" sheetId="28" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -63,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="79">
   <si>
     <t>action</t>
   </si>
@@ -282,6 +284,30 @@
   </si>
   <si>
     <t>failed-dateOfBirth</t>
+  </si>
+  <si>
+    <t>automated.test.rename@mail.com</t>
+  </si>
+  <si>
+    <t>Automated Name</t>
+  </si>
+  <si>
+    <t>Automated Rename</t>
+  </si>
+  <si>
+    <t>automatedRename</t>
+  </si>
+  <si>
+    <t>Rename</t>
+  </si>
+  <si>
+    <t>automated.test.check@mail.com</t>
+  </si>
+  <si>
+    <t>Automated check</t>
+  </si>
+  <si>
+    <t>signup-check</t>
   </si>
 </sst>
 </file>
@@ -402,15 +428,13 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -421,6 +445,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -837,7 +863,7 @@
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="19" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="11" t="s">
@@ -904,7 +930,7 @@
       <c r="X2" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="Y2" s="23" t="s">
+      <c r="Y2" s="21" t="s">
         <v>69</v>
       </c>
     </row>
@@ -921,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74A8D453-88BA-4430-BEC2-9D2C3EA6C8DE}">
   <dimension ref="A1:Y2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1017,11 +1043,11 @@
         <v>signup|action</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="17" customFormat="1">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:25" s="16" customFormat="1">
+      <c r="A2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1036,19 +1062,19 @@
       <c r="F2" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" t="s">
         <v>42</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>45</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>48</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>49</v>
       </c>
       <c r="L2" s="14" t="s">
@@ -1057,13 +1083,13 @@
       <c r="M2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="15" t="s">
         <v>41</v>
       </c>
       <c r="Q2" s="14" t="s">
@@ -1211,30 +1237,30 @@
       <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1353,30 +1379,30 @@
       <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1493,30 +1519,30 @@
       <c r="C2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>60</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1629,34 +1655,34 @@
       <c r="A2" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="11"/>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="18"/>
+      <c r="H2" s="18"/>
+      <c r="I2" s="18"/>
+      <c r="J2" s="18"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="18"/>
+      <c r="O2" s="18"/>
+      <c r="P2" s="18"/>
+      <c r="Q2" s="18"/>
+      <c r="R2" s="18"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="18"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="18"/>
+      <c r="X2" s="18"/>
+      <c r="Y2" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1763,11 +1789,11 @@
         <v>signup|action</v>
       </c>
     </row>
-    <row r="2" spans="1:25" s="17" customFormat="1">
-      <c r="A2" s="18" t="s">
+    <row r="2" spans="1:25" s="16" customFormat="1">
+      <c r="A2" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="20" t="s">
         <v>63</v>
       </c>
       <c r="C2" s="13" t="s">
@@ -1782,19 +1808,19 @@
       <c r="F2" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
         <v>63</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="16" t="s">
+      <c r="J2" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>49</v>
       </c>
       <c r="L2" s="14" t="s">
@@ -1803,13 +1829,13 @@
       <c r="M2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="N2" s="16" t="s">
+      <c r="N2" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="O2" s="16" t="s">
+      <c r="O2" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="P2" s="16" t="s">
+      <c r="P2" s="15" t="s">
         <v>41</v>
       </c>
       <c r="Q2" s="14" t="s">
@@ -1845,4 +1871,371 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{990B0AF9-7626-4249-B3F7-BB64A23F59EE}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" style="4" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="5" customWidth="1"/>
+    <col min="8" max="11" width="15.6328125" style="5" customWidth="1"/>
+    <col min="12" max="16" width="15.6328125" style="3" customWidth="1"/>
+    <col min="17" max="18" width="20.6328125" style="3" customWidth="1"/>
+    <col min="19" max="25" width="15.6328125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1">
+      <c r="A1" s="2" t="str" cm="1">
+        <f t="array" ref="A1:Y1">column_ref!A1:Y1</f>
+        <v>action</v>
+      </c>
+      <c r="B1" s="2" t="str">
+        <v>login|email</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <v>login|name</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <v>login|result</v>
+      </c>
+      <c r="E1" s="7" t="str">
+        <v>signup|title</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <v>signup|name</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <v>signup|email</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <v>signup|password</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <v>signup|day</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <v>signup|month</v>
+      </c>
+      <c r="K1" s="2" t="str">
+        <v>signup|year</v>
+      </c>
+      <c r="L1" s="2" t="str">
+        <v>signup|newsletter</v>
+      </c>
+      <c r="M1" s="2" t="str">
+        <v>signup|specialoffer</v>
+      </c>
+      <c r="N1" s="2" t="str">
+        <v>signup|firstname</v>
+      </c>
+      <c r="O1" s="2" t="str">
+        <v>signup|lastname</v>
+      </c>
+      <c r="P1" s="2" t="str">
+        <v>signup|company</v>
+      </c>
+      <c r="Q1" s="2" t="str">
+        <v>signup|address</v>
+      </c>
+      <c r="R1" s="2" t="str">
+        <v>signup|address2</v>
+      </c>
+      <c r="S1" s="2" t="str">
+        <v>signup|country</v>
+      </c>
+      <c r="T1" s="2" t="str">
+        <v>signup|state</v>
+      </c>
+      <c r="U1" s="2" t="str">
+        <v>signup|city</v>
+      </c>
+      <c r="V1" s="2" t="str">
+        <v>signup|zipcode</v>
+      </c>
+      <c r="W1" s="2" t="str">
+        <v>signup|mobile</v>
+      </c>
+      <c r="X1" s="2" t="str">
+        <v>signup|result</v>
+      </c>
+      <c r="Y1" s="2" t="str">
+        <v>signup|action</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="16" customFormat="1">
+      <c r="A2" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="B2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0DA1E833-B3FA-4223-B831-CC7D7BB451DB}">
+  <dimension ref="A1:Y2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="20.6328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="30.08984375" style="4" customWidth="1"/>
+    <col min="3" max="4" width="15.6328125" style="5" customWidth="1"/>
+    <col min="5" max="5" width="10.6328125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="17.81640625" style="5" customWidth="1"/>
+    <col min="7" max="7" width="25.6328125" style="5" customWidth="1"/>
+    <col min="8" max="11" width="15.6328125" style="5" customWidth="1"/>
+    <col min="12" max="16" width="15.6328125" style="3" customWidth="1"/>
+    <col min="17" max="18" width="20.6328125" style="3" customWidth="1"/>
+    <col min="19" max="25" width="15.6328125" style="3" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:25" s="1" customFormat="1">
+      <c r="A1" s="2" t="str" cm="1">
+        <f t="array" ref="A1:Y1">column_ref!A1:Y1</f>
+        <v>action</v>
+      </c>
+      <c r="B1" s="2" t="str">
+        <v>login|email</v>
+      </c>
+      <c r="C1" s="2" t="str">
+        <v>login|name</v>
+      </c>
+      <c r="D1" s="2" t="str">
+        <v>login|result</v>
+      </c>
+      <c r="E1" s="7" t="str">
+        <v>signup|title</v>
+      </c>
+      <c r="F1" s="2" t="str">
+        <v>signup|name</v>
+      </c>
+      <c r="G1" s="2" t="str">
+        <v>signup|email</v>
+      </c>
+      <c r="H1" s="2" t="str">
+        <v>signup|password</v>
+      </c>
+      <c r="I1" s="2" t="str">
+        <v>signup|day</v>
+      </c>
+      <c r="J1" s="2" t="str">
+        <v>signup|month</v>
+      </c>
+      <c r="K1" s="2" t="str">
+        <v>signup|year</v>
+      </c>
+      <c r="L1" s="2" t="str">
+        <v>signup|newsletter</v>
+      </c>
+      <c r="M1" s="2" t="str">
+        <v>signup|specialoffer</v>
+      </c>
+      <c r="N1" s="2" t="str">
+        <v>signup|firstname</v>
+      </c>
+      <c r="O1" s="2" t="str">
+        <v>signup|lastname</v>
+      </c>
+      <c r="P1" s="2" t="str">
+        <v>signup|company</v>
+      </c>
+      <c r="Q1" s="2" t="str">
+        <v>signup|address</v>
+      </c>
+      <c r="R1" s="2" t="str">
+        <v>signup|address2</v>
+      </c>
+      <c r="S1" s="2" t="str">
+        <v>signup|country</v>
+      </c>
+      <c r="T1" s="2" t="str">
+        <v>signup|state</v>
+      </c>
+      <c r="U1" s="2" t="str">
+        <v>signup|city</v>
+      </c>
+      <c r="V1" s="2" t="str">
+        <v>signup|zipcode</v>
+      </c>
+      <c r="W1" s="2" t="str">
+        <v>signup|mobile</v>
+      </c>
+      <c r="X1" s="2" t="str">
+        <v>signup|result</v>
+      </c>
+      <c r="Y1" s="2" t="str">
+        <v>signup|action</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="16" customFormat="1">
+      <c r="A2" s="17" t="s">
+        <v>78</v>
+      </c>
+      <c r="B2" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G2" t="s">
+        <v>42</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="I2" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="J2" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="L2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="M2" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="N2" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="O2" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q2" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="R2" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="S2" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="T2" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="U2" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="V2" s="13" t="s">
+        <v>55</v>
+      </c>
+      <c r="W2" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="X2" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="Y2" s="14" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{4B533301-368F-462E-A914-1974AF34298D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>